<commit_message>
Archivo send_documents por fin jala, excel enviado
</commit_message>
<xml_diff>
--- a/BabaBooey.xlsx
+++ b/BabaBooey.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\OneDrive\Documentos\PythonProjects\Python\eigenseed_telegrambots\EigenSeedTelegram\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B1573C-1027-4513-9F9C-DAE2C6139662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +72,88 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>159835</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7508209" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926FEFCB-4D2D-055D-4F3C-7D9D1F15A868}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3416320" y="1622875"/>
+          <a:ext cx="7508209" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="soft" dir="t">
+              <a:rot lat="0" lon="0" rev="15600000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d extrusionH="57150" prstMaterial="softEdge">
+            <a:bevelT w="25400" h="38100"/>
+          </a:sp3d>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="5400" b="1" cap="none" spc="0">
+              <a:ln/>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>CHINGA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="5400" b="1" cap="none" spc="0" baseline="0">
+              <a:ln/>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> TU MADRE, YURI</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="5400" b="1" cap="none" spc="0">
+            <a:ln/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +418,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>